<commit_message>
grouping, concatenation , merging
</commit_message>
<xml_diff>
--- a/E_post2.xlsx
+++ b/E_post2.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\786\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185C9BAD-9AB9-4B18-84B7-724F26E5D4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -46,8 +52,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +116,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -154,7 +168,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -188,6 +202,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -222,9 +237,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -397,14 +413,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5248</v>
       </c>
@@ -462,18 +491,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4294</v>
       </c>
       <c r="B3">
-        <v>9507</v>
+        <v>6090</v>
       </c>
       <c r="C3">
         <v>4798</v>
       </c>
       <c r="D3">
-        <v>1551</v>
+        <v>3128</v>
       </c>
       <c r="E3">
         <v>3826855548337</v>
@@ -491,18 +520,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2550</v>
       </c>
       <c r="B4">
-        <v>9001</v>
+        <v>6090</v>
       </c>
       <c r="C4">
         <v>3494</v>
       </c>
       <c r="D4">
-        <v>4795</v>
+        <v>3128</v>
       </c>
       <c r="E4">
         <v>2698853863428</v>
@@ -520,18 +549,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1420</v>
       </c>
       <c r="B5">
-        <v>8337</v>
+        <v>6090</v>
       </c>
       <c r="C5">
         <v>2778</v>
       </c>
       <c r="D5">
-        <v>5050</v>
+        <v>3128</v>
       </c>
       <c r="E5">
         <v>8791112114856</v>
@@ -549,18 +578,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>9390</v>
       </c>
       <c r="B6">
-        <v>9443</v>
+        <v>6090</v>
       </c>
       <c r="C6">
         <v>4064</v>
       </c>
       <c r="D6">
-        <v>7886</v>
+        <v>3128</v>
       </c>
       <c r="E6">
         <v>6224067416477</v>
@@ -578,18 +607,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>9437</v>
       </c>
       <c r="B7">
-        <v>3172</v>
+        <v>6090</v>
       </c>
       <c r="C7">
         <v>2619</v>
       </c>
       <c r="D7">
-        <v>5653</v>
+        <v>3128</v>
       </c>
       <c r="E7">
         <v>4268882408949</v>
@@ -607,12 +636,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6160</v>
       </c>
       <c r="B8">
-        <v>4246</v>
+        <v>6090</v>
       </c>
       <c r="C8">
         <v>4366</v>
@@ -636,7 +665,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3342</v>
       </c>
@@ -647,7 +676,7 @@
         <v>1965</v>
       </c>
       <c r="D9">
-        <v>7462</v>
+        <v>6962</v>
       </c>
       <c r="E9">
         <v>8347967283187</v>
@@ -665,18 +694,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3949</v>
       </c>
       <c r="B10">
-        <v>7682</v>
+        <v>3182</v>
       </c>
       <c r="C10">
         <v>1954</v>
       </c>
       <c r="D10">
-        <v>9400</v>
+        <v>6962</v>
       </c>
       <c r="E10">
         <v>3568567306976</v>
@@ -694,18 +723,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2837</v>
       </c>
       <c r="B11">
-        <v>9232</v>
+        <v>3182</v>
       </c>
       <c r="C11">
         <v>3858</v>
       </c>
       <c r="D11">
-        <v>4211</v>
+        <v>6962</v>
       </c>
       <c r="E11">
         <v>3871937225010</v>
@@ -723,18 +752,18 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>6298</v>
       </c>
       <c r="B12">
-        <v>3826</v>
+        <v>3182</v>
       </c>
       <c r="C12">
         <v>9969</v>
       </c>
       <c r="D12">
-        <v>6031</v>
+        <v>6962</v>
       </c>
       <c r="E12">
         <v>3291842849301</v>
@@ -752,18 +781,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>7511</v>
       </c>
       <c r="B13">
-        <v>1631</v>
+        <v>3182</v>
       </c>
       <c r="C13">
         <v>9649</v>
       </c>
       <c r="D13">
-        <v>4171</v>
+        <v>6962</v>
       </c>
       <c r="E13">
         <v>5545543570785</v>
@@ -781,18 +810,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>6232</v>
       </c>
       <c r="B14">
-        <v>8573</v>
+        <v>3182</v>
       </c>
       <c r="C14">
         <v>3267</v>
       </c>
       <c r="D14">
-        <v>2013</v>
+        <v>6962</v>
       </c>
       <c r="E14">
         <v>5845053788768</v>
@@ -810,7 +839,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>4533</v>
       </c>
@@ -821,7 +850,7 @@
         <v>3999</v>
       </c>
       <c r="D15">
-        <v>1201</v>
+        <v>6962</v>
       </c>
       <c r="E15">
         <v>9633918823464</v>
@@ -839,12 +868,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>4990</v>
       </c>
       <c r="B16">
-        <v>7710</v>
+        <v>1666</v>
       </c>
       <c r="C16">
         <v>4354</v>
@@ -868,18 +897,18 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>8321</v>
       </c>
       <c r="B17">
-        <v>3001</v>
+        <v>1666</v>
       </c>
       <c r="C17">
         <v>7497</v>
       </c>
       <c r="D17">
-        <v>4133</v>
+        <v>1892</v>
       </c>
       <c r="E17">
         <v>8719732747518</v>
@@ -897,18 +926,18 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>6213</v>
       </c>
       <c r="B18">
-        <v>2069</v>
+        <v>1666</v>
       </c>
       <c r="C18">
         <v>8932</v>
       </c>
       <c r="D18">
-        <v>5746</v>
+        <v>1892</v>
       </c>
       <c r="E18">
         <v>3391874944101</v>
@@ -926,18 +955,18 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>5686</v>
       </c>
       <c r="B19">
-        <v>9623</v>
+        <v>1666</v>
       </c>
       <c r="C19">
         <v>1859</v>
       </c>
       <c r="D19">
-        <v>2449</v>
+        <v>1892</v>
       </c>
       <c r="E19">
         <v>2205315292500</v>
@@ -955,18 +984,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1356</v>
       </c>
       <c r="B20">
-        <v>8799</v>
+        <v>1666</v>
       </c>
       <c r="C20">
         <v>3733</v>
       </c>
       <c r="D20">
-        <v>9702</v>
+        <v>1892</v>
       </c>
       <c r="E20">
         <v>4425357155589</v>
@@ -984,18 +1013,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>8967</v>
       </c>
       <c r="B21">
-        <v>1942</v>
+        <v>1666</v>
       </c>
       <c r="C21">
         <v>8004</v>
       </c>
       <c r="D21">
-        <v>3964</v>
+        <v>1892</v>
       </c>
       <c r="E21">
         <v>7019296534561</v>

</xml_diff>